<commit_message>
View Html Report - View Stats - View Area Stats - Failed Skipped And Passing Feature Stats View Html Report - View Stats - View Area Stats - Failed Skipped And Passing Scenario Stats View Html Report - View Stats - View Area Stats - Failed Skipped And Passing Steps Stats
</commit_message>
<xml_diff>
--- a/xBDD/test/xBDD.Reporting.Test/Features/ViewHtmlReport/ViewStats/FullTestRunAllOutcomesStats.xlsx
+++ b/xBDD/test/xBDD.Reporting.Test/Features/ViewHtmlReport/ViewStats/FullTestRunAllOutcomesStats.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8520" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11500" windowHeight="8470" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Skips And Fails" sheetId="2" r:id="rId1"/>
@@ -22,9 +22,9 @@
   </definedNames>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId5"/>
-    <pivotCache cacheId="10" r:id="rId6"/>
-    <pivotCache cacheId="22" r:id="rId7"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
+    <pivotCache cacheId="1" r:id="rId6"/>
+    <pivotCache cacheId="4" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="23">
   <si>
     <t>Area</t>
   </si>
@@ -90,13 +90,28 @@
   <si>
     <t>Count of StepOutcome</t>
   </si>
+  <si>
+    <t>Areas 1</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Features</t>
+  </si>
+  <si>
+    <t>Scenarios</t>
+  </si>
+  <si>
+    <t>Steps</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="175" formatCode="0.0000000000000%"/>
+    <numFmt numFmtId="164" formatCode="0.0000000000000%"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -140,7 +155,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -216,7 +231,11 @@
   </cacheSource>
   <cacheFields count="8">
     <cacheField name="AreaOutcome" numFmtId="0">
-      <sharedItems/>
+      <sharedItems count="3">
+        <s v="Passing"/>
+        <s v="Skipped"/>
+        <s v="Failed"/>
+      </sharedItems>
     </cacheField>
     <cacheField name="Area" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="3"/>
@@ -410,7 +429,7 @@
 <file path=xl/pivotCache/pivotCacheRecords3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="81">
   <r>
-    <s v="Passing"/>
+    <x v="0"/>
     <n v="1"/>
     <s v="Passing"/>
     <n v="1"/>
@@ -420,7 +439,7 @@
     <n v="1"/>
   </r>
   <r>
-    <s v="Passing"/>
+    <x v="0"/>
     <n v="1"/>
     <s v="Passing"/>
     <n v="1"/>
@@ -430,7 +449,7 @@
     <n v="2"/>
   </r>
   <r>
-    <s v="Passing"/>
+    <x v="0"/>
     <n v="1"/>
     <s v="Passing"/>
     <n v="1"/>
@@ -440,7 +459,7 @@
     <n v="3"/>
   </r>
   <r>
-    <s v="Passing"/>
+    <x v="0"/>
     <n v="1"/>
     <s v="Passing"/>
     <n v="1"/>
@@ -450,7 +469,7 @@
     <n v="4"/>
   </r>
   <r>
-    <s v="Passing"/>
+    <x v="0"/>
     <n v="1"/>
     <s v="Passing"/>
     <n v="1"/>
@@ -460,7 +479,7 @@
     <n v="5"/>
   </r>
   <r>
-    <s v="Passing"/>
+    <x v="0"/>
     <n v="1"/>
     <s v="Passing"/>
     <n v="1"/>
@@ -470,7 +489,7 @@
     <n v="6"/>
   </r>
   <r>
-    <s v="Passing"/>
+    <x v="0"/>
     <n v="1"/>
     <s v="Passing"/>
     <n v="1"/>
@@ -480,7 +499,7 @@
     <n v="7"/>
   </r>
   <r>
-    <s v="Passing"/>
+    <x v="0"/>
     <n v="1"/>
     <s v="Passing"/>
     <n v="1"/>
@@ -490,7 +509,7 @@
     <n v="8"/>
   </r>
   <r>
-    <s v="Passing"/>
+    <x v="0"/>
     <n v="1"/>
     <s v="Passing"/>
     <n v="1"/>
@@ -500,7 +519,7 @@
     <n v="9"/>
   </r>
   <r>
-    <s v="Passing"/>
+    <x v="0"/>
     <n v="1"/>
     <s v="Passing"/>
     <n v="2"/>
@@ -510,7 +529,7 @@
     <n v="10"/>
   </r>
   <r>
-    <s v="Passing"/>
+    <x v="0"/>
     <n v="1"/>
     <s v="Passing"/>
     <n v="2"/>
@@ -520,7 +539,7 @@
     <n v="11"/>
   </r>
   <r>
-    <s v="Passing"/>
+    <x v="0"/>
     <n v="1"/>
     <s v="Passing"/>
     <n v="2"/>
@@ -530,7 +549,7 @@
     <n v="12"/>
   </r>
   <r>
-    <s v="Passing"/>
+    <x v="0"/>
     <n v="1"/>
     <s v="Passing"/>
     <n v="2"/>
@@ -540,7 +559,7 @@
     <n v="13"/>
   </r>
   <r>
-    <s v="Passing"/>
+    <x v="0"/>
     <n v="1"/>
     <s v="Passing"/>
     <n v="2"/>
@@ -550,7 +569,7 @@
     <n v="14"/>
   </r>
   <r>
-    <s v="Passing"/>
+    <x v="0"/>
     <n v="1"/>
     <s v="Passing"/>
     <n v="2"/>
@@ -560,7 +579,7 @@
     <n v="15"/>
   </r>
   <r>
-    <s v="Passing"/>
+    <x v="0"/>
     <n v="1"/>
     <s v="Passing"/>
     <n v="2"/>
@@ -570,7 +589,7 @@
     <n v="16"/>
   </r>
   <r>
-    <s v="Passing"/>
+    <x v="0"/>
     <n v="1"/>
     <s v="Passing"/>
     <n v="2"/>
@@ -580,7 +599,7 @@
     <n v="17"/>
   </r>
   <r>
-    <s v="Passing"/>
+    <x v="0"/>
     <n v="1"/>
     <s v="Passing"/>
     <n v="2"/>
@@ -590,7 +609,7 @@
     <n v="18"/>
   </r>
   <r>
-    <s v="Passing"/>
+    <x v="0"/>
     <n v="1"/>
     <s v="Passing"/>
     <n v="3"/>
@@ -600,7 +619,7 @@
     <n v="19"/>
   </r>
   <r>
-    <s v="Passing"/>
+    <x v="0"/>
     <n v="1"/>
     <s v="Passing"/>
     <n v="3"/>
@@ -610,7 +629,7 @@
     <n v="20"/>
   </r>
   <r>
-    <s v="Passing"/>
+    <x v="0"/>
     <n v="1"/>
     <s v="Passing"/>
     <n v="3"/>
@@ -620,7 +639,7 @@
     <n v="21"/>
   </r>
   <r>
-    <s v="Passing"/>
+    <x v="0"/>
     <n v="1"/>
     <s v="Passing"/>
     <n v="3"/>
@@ -630,7 +649,7 @@
     <n v="22"/>
   </r>
   <r>
-    <s v="Passing"/>
+    <x v="0"/>
     <n v="1"/>
     <s v="Passing"/>
     <n v="3"/>
@@ -640,7 +659,7 @@
     <n v="23"/>
   </r>
   <r>
-    <s v="Passing"/>
+    <x v="0"/>
     <n v="1"/>
     <s v="Passing"/>
     <n v="3"/>
@@ -650,7 +669,7 @@
     <n v="24"/>
   </r>
   <r>
-    <s v="Passing"/>
+    <x v="0"/>
     <n v="1"/>
     <s v="Passing"/>
     <n v="3"/>
@@ -660,7 +679,7 @@
     <n v="25"/>
   </r>
   <r>
-    <s v="Passing"/>
+    <x v="0"/>
     <n v="1"/>
     <s v="Passing"/>
     <n v="3"/>
@@ -670,7 +689,7 @@
     <n v="26"/>
   </r>
   <r>
-    <s v="Passing"/>
+    <x v="0"/>
     <n v="1"/>
     <s v="Passing"/>
     <n v="3"/>
@@ -680,7 +699,7 @@
     <n v="27"/>
   </r>
   <r>
-    <s v="Skipped"/>
+    <x v="1"/>
     <n v="2"/>
     <s v="Skipped"/>
     <n v="4"/>
@@ -690,7 +709,7 @@
     <n v="28"/>
   </r>
   <r>
-    <s v="Skipped"/>
+    <x v="1"/>
     <n v="2"/>
     <s v="Skipped"/>
     <n v="4"/>
@@ -700,7 +719,7 @@
     <n v="29"/>
   </r>
   <r>
-    <s v="Skipped"/>
+    <x v="1"/>
     <n v="2"/>
     <s v="Skipped"/>
     <n v="4"/>
@@ -710,7 +729,7 @@
     <n v="30"/>
   </r>
   <r>
-    <s v="Skipped"/>
+    <x v="1"/>
     <n v="2"/>
     <s v="Skipped"/>
     <n v="4"/>
@@ -720,7 +739,7 @@
     <n v="31"/>
   </r>
   <r>
-    <s v="Skipped"/>
+    <x v="1"/>
     <n v="2"/>
     <s v="Skipped"/>
     <n v="4"/>
@@ -730,7 +749,7 @@
     <n v="32"/>
   </r>
   <r>
-    <s v="Skipped"/>
+    <x v="1"/>
     <n v="2"/>
     <s v="Skipped"/>
     <n v="4"/>
@@ -740,7 +759,7 @@
     <n v="33"/>
   </r>
   <r>
-    <s v="Skipped"/>
+    <x v="1"/>
     <n v="2"/>
     <s v="Skipped"/>
     <n v="4"/>
@@ -750,7 +769,7 @@
     <n v="34"/>
   </r>
   <r>
-    <s v="Skipped"/>
+    <x v="1"/>
     <n v="2"/>
     <s v="Skipped"/>
     <n v="4"/>
@@ -760,7 +779,7 @@
     <n v="35"/>
   </r>
   <r>
-    <s v="Skipped"/>
+    <x v="1"/>
     <n v="2"/>
     <s v="Skipped"/>
     <n v="4"/>
@@ -770,7 +789,7 @@
     <n v="36"/>
   </r>
   <r>
-    <s v="Skipped"/>
+    <x v="1"/>
     <n v="2"/>
     <s v="Skipped"/>
     <n v="5"/>
@@ -780,7 +799,7 @@
     <n v="37"/>
   </r>
   <r>
-    <s v="Skipped"/>
+    <x v="1"/>
     <n v="2"/>
     <s v="Skipped"/>
     <n v="5"/>
@@ -790,7 +809,7 @@
     <n v="38"/>
   </r>
   <r>
-    <s v="Skipped"/>
+    <x v="1"/>
     <n v="2"/>
     <s v="Skipped"/>
     <n v="5"/>
@@ -800,7 +819,7 @@
     <n v="39"/>
   </r>
   <r>
-    <s v="Skipped"/>
+    <x v="1"/>
     <n v="2"/>
     <s v="Skipped"/>
     <n v="5"/>
@@ -810,7 +829,7 @@
     <n v="40"/>
   </r>
   <r>
-    <s v="Skipped"/>
+    <x v="1"/>
     <n v="2"/>
     <s v="Skipped"/>
     <n v="5"/>
@@ -820,7 +839,7 @@
     <n v="41"/>
   </r>
   <r>
-    <s v="Skipped"/>
+    <x v="1"/>
     <n v="2"/>
     <s v="Skipped"/>
     <n v="5"/>
@@ -830,7 +849,7 @@
     <n v="42"/>
   </r>
   <r>
-    <s v="Skipped"/>
+    <x v="1"/>
     <n v="2"/>
     <s v="Skipped"/>
     <n v="5"/>
@@ -840,7 +859,7 @@
     <n v="43"/>
   </r>
   <r>
-    <s v="Skipped"/>
+    <x v="1"/>
     <n v="2"/>
     <s v="Skipped"/>
     <n v="5"/>
@@ -850,7 +869,7 @@
     <n v="44"/>
   </r>
   <r>
-    <s v="Skipped"/>
+    <x v="1"/>
     <n v="2"/>
     <s v="Skipped"/>
     <n v="5"/>
@@ -860,7 +879,7 @@
     <n v="45"/>
   </r>
   <r>
-    <s v="Skipped"/>
+    <x v="1"/>
     <n v="2"/>
     <s v="Passing"/>
     <n v="6"/>
@@ -870,7 +889,7 @@
     <n v="46"/>
   </r>
   <r>
-    <s v="Skipped"/>
+    <x v="1"/>
     <n v="2"/>
     <s v="Passing"/>
     <n v="6"/>
@@ -880,7 +899,7 @@
     <n v="47"/>
   </r>
   <r>
-    <s v="Skipped"/>
+    <x v="1"/>
     <n v="2"/>
     <s v="Passing"/>
     <n v="6"/>
@@ -890,7 +909,7 @@
     <n v="48"/>
   </r>
   <r>
-    <s v="Skipped"/>
+    <x v="1"/>
     <n v="2"/>
     <s v="Passing"/>
     <n v="6"/>
@@ -900,7 +919,7 @@
     <n v="49"/>
   </r>
   <r>
-    <s v="Skipped"/>
+    <x v="1"/>
     <n v="2"/>
     <s v="Passing"/>
     <n v="6"/>
@@ -910,7 +929,7 @@
     <n v="50"/>
   </r>
   <r>
-    <s v="Skipped"/>
+    <x v="1"/>
     <n v="2"/>
     <s v="Passing"/>
     <n v="6"/>
@@ -920,7 +939,7 @@
     <n v="51"/>
   </r>
   <r>
-    <s v="Skipped"/>
+    <x v="1"/>
     <n v="2"/>
     <s v="Passing"/>
     <n v="6"/>
@@ -930,7 +949,7 @@
     <n v="52"/>
   </r>
   <r>
-    <s v="Skipped"/>
+    <x v="1"/>
     <n v="2"/>
     <s v="Passing"/>
     <n v="6"/>
@@ -940,7 +959,7 @@
     <n v="53"/>
   </r>
   <r>
-    <s v="Skipped"/>
+    <x v="1"/>
     <n v="2"/>
     <s v="Passing"/>
     <n v="6"/>
@@ -950,7 +969,7 @@
     <n v="54"/>
   </r>
   <r>
-    <s v="Failed"/>
+    <x v="2"/>
     <n v="3"/>
     <s v="Failed"/>
     <n v="7"/>
@@ -960,7 +979,7 @@
     <n v="55"/>
   </r>
   <r>
-    <s v="Failed"/>
+    <x v="2"/>
     <n v="3"/>
     <s v="Failed"/>
     <n v="7"/>
@@ -970,7 +989,7 @@
     <n v="56"/>
   </r>
   <r>
-    <s v="Failed"/>
+    <x v="2"/>
     <n v="3"/>
     <s v="Failed"/>
     <n v="7"/>
@@ -980,7 +999,7 @@
     <n v="57"/>
   </r>
   <r>
-    <s v="Failed"/>
+    <x v="2"/>
     <n v="3"/>
     <s v="Failed"/>
     <n v="7"/>
@@ -990,7 +1009,7 @@
     <n v="58"/>
   </r>
   <r>
-    <s v="Failed"/>
+    <x v="2"/>
     <n v="3"/>
     <s v="Failed"/>
     <n v="7"/>
@@ -1000,7 +1019,7 @@
     <n v="59"/>
   </r>
   <r>
-    <s v="Failed"/>
+    <x v="2"/>
     <n v="3"/>
     <s v="Failed"/>
     <n v="7"/>
@@ -1010,7 +1029,7 @@
     <n v="60"/>
   </r>
   <r>
-    <s v="Failed"/>
+    <x v="2"/>
     <n v="3"/>
     <s v="Failed"/>
     <n v="7"/>
@@ -1020,7 +1039,7 @@
     <n v="61"/>
   </r>
   <r>
-    <s v="Failed"/>
+    <x v="2"/>
     <n v="3"/>
     <s v="Failed"/>
     <n v="7"/>
@@ -1030,7 +1049,7 @@
     <n v="62"/>
   </r>
   <r>
-    <s v="Failed"/>
+    <x v="2"/>
     <n v="3"/>
     <s v="Failed"/>
     <n v="7"/>
@@ -1040,7 +1059,7 @@
     <n v="63"/>
   </r>
   <r>
-    <s v="Failed"/>
+    <x v="2"/>
     <n v="3"/>
     <s v="Skipped"/>
     <n v="8"/>
@@ -1050,7 +1069,7 @@
     <n v="64"/>
   </r>
   <r>
-    <s v="Failed"/>
+    <x v="2"/>
     <n v="3"/>
     <s v="Skipped"/>
     <n v="8"/>
@@ -1060,7 +1079,7 @@
     <n v="65"/>
   </r>
   <r>
-    <s v="Failed"/>
+    <x v="2"/>
     <n v="3"/>
     <s v="Skipped"/>
     <n v="8"/>
@@ -1070,7 +1089,7 @@
     <n v="66"/>
   </r>
   <r>
-    <s v="Failed"/>
+    <x v="2"/>
     <n v="3"/>
     <s v="Skipped"/>
     <n v="8"/>
@@ -1080,7 +1099,7 @@
     <n v="67"/>
   </r>
   <r>
-    <s v="Failed"/>
+    <x v="2"/>
     <n v="3"/>
     <s v="Skipped"/>
     <n v="8"/>
@@ -1090,7 +1109,7 @@
     <n v="68"/>
   </r>
   <r>
-    <s v="Failed"/>
+    <x v="2"/>
     <n v="3"/>
     <s v="Skipped"/>
     <n v="8"/>
@@ -1100,7 +1119,7 @@
     <n v="69"/>
   </r>
   <r>
-    <s v="Failed"/>
+    <x v="2"/>
     <n v="3"/>
     <s v="Skipped"/>
     <n v="8"/>
@@ -1110,7 +1129,7 @@
     <n v="70"/>
   </r>
   <r>
-    <s v="Failed"/>
+    <x v="2"/>
     <n v="3"/>
     <s v="Skipped"/>
     <n v="8"/>
@@ -1120,7 +1139,7 @@
     <n v="71"/>
   </r>
   <r>
-    <s v="Failed"/>
+    <x v="2"/>
     <n v="3"/>
     <s v="Skipped"/>
     <n v="8"/>
@@ -1130,7 +1149,7 @@
     <n v="72"/>
   </r>
   <r>
-    <s v="Failed"/>
+    <x v="2"/>
     <n v="3"/>
     <s v="Passing"/>
     <n v="9"/>
@@ -1140,7 +1159,7 @@
     <n v="73"/>
   </r>
   <r>
-    <s v="Failed"/>
+    <x v="2"/>
     <n v="3"/>
     <s v="Passing"/>
     <n v="9"/>
@@ -1150,7 +1169,7 @@
     <n v="74"/>
   </r>
   <r>
-    <s v="Failed"/>
+    <x v="2"/>
     <n v="3"/>
     <s v="Passing"/>
     <n v="9"/>
@@ -1160,7 +1179,7 @@
     <n v="75"/>
   </r>
   <r>
-    <s v="Failed"/>
+    <x v="2"/>
     <n v="3"/>
     <s v="Passing"/>
     <n v="9"/>
@@ -1170,7 +1189,7 @@
     <n v="76"/>
   </r>
   <r>
-    <s v="Failed"/>
+    <x v="2"/>
     <n v="3"/>
     <s v="Passing"/>
     <n v="9"/>
@@ -1180,7 +1199,7 @@
     <n v="77"/>
   </r>
   <r>
-    <s v="Failed"/>
+    <x v="2"/>
     <n v="3"/>
     <s v="Passing"/>
     <n v="9"/>
@@ -1190,7 +1209,7 @@
     <n v="78"/>
   </r>
   <r>
-    <s v="Failed"/>
+    <x v="2"/>
     <n v="3"/>
     <s v="Passing"/>
     <n v="9"/>
@@ -1200,7 +1219,7 @@
     <n v="79"/>
   </r>
   <r>
-    <s v="Failed"/>
+    <x v="2"/>
     <n v="3"/>
     <s v="Passing"/>
     <n v="9"/>
@@ -1210,7 +1229,7 @@
     <n v="80"/>
   </r>
   <r>
-    <s v="Failed"/>
+    <x v="2"/>
     <n v="3"/>
     <s v="Passing"/>
     <n v="9"/>
@@ -1223,7 +1242,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A12:E14" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisCol" showAll="0">
@@ -1269,7 +1288,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A30:E32" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisCol" dataField="1" showAll="0">
@@ -1315,7 +1334,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="22" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A87:E89" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField showAll="0"/>
@@ -1696,8 +1715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2143,18 +2162,17 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:I90"/>
+  <dimension ref="A1:I99"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D90" sqref="D90"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="4" width="18" customWidth="1"/>
+    <col min="2" max="4" width="18" customWidth="1"/>
     <col min="5" max="5" width="10.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2904,7 +2922,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>5</v>
       </c>
@@ -2930,7 +2948,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>5</v>
       </c>
@@ -2956,7 +2974,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>5</v>
       </c>
@@ -2982,7 +3000,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -3008,7 +3026,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>5</v>
       </c>
@@ -3034,7 +3052,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>5</v>
       </c>
@@ -3138,7 +3156,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>5</v>
       </c>
@@ -3164,7 +3182,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>5</v>
       </c>
@@ -3190,7 +3208,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>5</v>
       </c>
@@ -3216,7 +3234,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>5</v>
       </c>
@@ -3242,7 +3260,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>5</v>
       </c>
@@ -3268,7 +3286,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>5</v>
       </c>
@@ -3606,7 +3624,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>6</v>
       </c>
@@ -3632,7 +3650,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>6</v>
       </c>
@@ -3658,7 +3676,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>6</v>
       </c>
@@ -3762,7 +3780,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>6</v>
       </c>
@@ -3788,7 +3806,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>6</v>
       </c>
@@ -3814,7 +3832,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>6</v>
       </c>
@@ -3996,7 +4014,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>6</v>
       </c>
@@ -4022,7 +4040,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>6</v>
       </c>
@@ -4048,7 +4066,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="75" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>6</v>
       </c>
@@ -4074,7 +4092,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>6</v>
       </c>
@@ -4100,7 +4118,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>6</v>
       </c>
@@ -4126,7 +4144,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>6</v>
       </c>
@@ -4152,7 +4170,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>6</v>
       </c>
@@ -4178,7 +4196,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>6</v>
       </c>
@@ -4204,7 +4222,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>6</v>
       </c>
@@ -4230,7 +4248,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>6</v>
       </c>
@@ -4256,7 +4274,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>6</v>
       </c>
@@ -4282,7 +4300,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>6</v>
       </c>
@@ -4358,11 +4376,121 @@
         <v>0.27160493827160492</v>
       </c>
     </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>18</v>
+      </c>
+      <c r="B93" t="s">
+        <v>4</v>
+      </c>
+      <c r="C93" t="s">
+        <v>5</v>
+      </c>
+      <c r="D93" t="s">
+        <v>6</v>
+      </c>
+      <c r="E93" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>20</v>
+      </c>
+      <c r="B94">
+        <v>1</v>
+      </c>
+      <c r="C94">
+        <v>1</v>
+      </c>
+      <c r="D94">
+        <v>1</v>
+      </c>
+      <c r="E94">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B95" s="4">
+        <f>B94/E94</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C95" s="4">
+        <f>C94/E94</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D95" s="4">
+        <f>D94/E94</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>21</v>
+      </c>
+      <c r="B96">
+        <v>5</v>
+      </c>
+      <c r="C96">
+        <v>3</v>
+      </c>
+      <c r="D96">
+        <v>1</v>
+      </c>
+      <c r="E96">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B97" s="4">
+        <f>B96/E96</f>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="C97" s="4">
+        <f>C96/E96</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D97" s="4">
+        <f>D96/E96</f>
+        <v>0.1111111111111111</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>22</v>
+      </c>
+      <c r="B98">
+        <v>16</v>
+      </c>
+      <c r="C98">
+        <v>10</v>
+      </c>
+      <c r="D98">
+        <v>1</v>
+      </c>
+      <c r="E98">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B99" s="4">
+        <f>B98/E98</f>
+        <v>0.59259259259259256</v>
+      </c>
+      <c r="C99" s="4">
+        <f>C98/E98</f>
+        <v>0.37037037037037035</v>
+      </c>
+      <c r="D99" s="4">
+        <f>D98/E98</f>
+        <v>3.7037037037037035E-2</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:H84">
-    <filterColumn colId="4">
+    <filterColumn colId="1">
       <filters>
-        <filter val="Skipped"/>
+        <filter val="3"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
View Html Report - View Stats - View Test Run Stats - Area Stats No Areas
</commit_message>
<xml_diff>
--- a/xBDD/test/xBDD.Reporting.Test/Features/ViewHtmlReport/ViewStats/FullTestRunAllOutcomesStats.xlsx
+++ b/xBDD/test/xBDD.Reporting.Test/Features/ViewHtmlReport/ViewStats/FullTestRunAllOutcomesStats.xlsx
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Steps!$A$3:$H$84</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" calcMode="manual"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId5"/>
     <pivotCache cacheId="1" r:id="rId6"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="24">
   <si>
     <t>Area</t>
   </si>
@@ -91,9 +91,6 @@
     <t>Count of StepOutcome</t>
   </si>
   <si>
-    <t>Areas 1</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -104,6 +101,12 @@
   </si>
   <si>
     <t>Steps</t>
+  </si>
+  <si>
+    <t>Area 3</t>
+  </si>
+  <si>
+    <t>Feature 7</t>
   </si>
 </sst>
 </file>
@@ -2162,11 +2165,11 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:I99"/>
+  <dimension ref="A1:I105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D99" sqref="D99"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G58" sqref="G58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4378,24 +4381,24 @@
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
+        <v>22</v>
+      </c>
+      <c r="B93" t="s">
+        <v>4</v>
+      </c>
+      <c r="C93" t="s">
+        <v>5</v>
+      </c>
+      <c r="D93" t="s">
+        <v>6</v>
+      </c>
+      <c r="E93" t="s">
         <v>18</v>
-      </c>
-      <c r="B93" t="s">
-        <v>4</v>
-      </c>
-      <c r="C93" t="s">
-        <v>5</v>
-      </c>
-      <c r="D93" t="s">
-        <v>6</v>
-      </c>
-      <c r="E93" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B94">
         <v>1</v>
@@ -4426,7 +4429,7 @@
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B96">
         <v>5</v>
@@ -4457,7 +4460,7 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B98">
         <v>16</v>
@@ -4484,6 +4487,85 @@
       <c r="D99" s="4">
         <f>D98/E98</f>
         <v>3.7037037037037035E-2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>23</v>
+      </c>
+      <c r="B101" t="s">
+        <v>4</v>
+      </c>
+      <c r="C101" t="s">
+        <v>5</v>
+      </c>
+      <c r="D101" t="s">
+        <v>6</v>
+      </c>
+      <c r="E101" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>20</v>
+      </c>
+      <c r="B102">
+        <v>1</v>
+      </c>
+      <c r="C102">
+        <v>1</v>
+      </c>
+      <c r="D102">
+        <v>1</v>
+      </c>
+      <c r="E102">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B103" s="4">
+        <f>B102/E102</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C103" s="4">
+        <f>C102/E102</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D103" s="4">
+        <f>D102/E102</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>21</v>
+      </c>
+      <c r="B104">
+        <v>4</v>
+      </c>
+      <c r="C104">
+        <v>4</v>
+      </c>
+      <c r="D104">
+        <v>1</v>
+      </c>
+      <c r="E104">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B105" s="4">
+        <f>B104/E104</f>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="C105" s="4">
+        <f>C104/E104</f>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="D105" s="4">
+        <f>D104/E104</f>
+        <v>0.1111111111111111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>